<commit_message>
Req 3 Logic requirement
</commit_message>
<xml_diff>
--- a/ElectronFrontend/assets/archivo.xlsx
+++ b/ElectronFrontend/assets/archivo.xlsx
@@ -1,96 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BFA872-AB73-4A00-8441-8D945D48FA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Hoja 1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Vehicle</t>
-  </si>
-  <si>
-    <t>Start time</t>
-  </si>
-  <si>
-    <t>End time</t>
+    <t>Vehiculo</t>
+  </si>
+  <si>
+    <t>Dia inicio</t>
+  </si>
+  <si>
+    <t>Hora inicio</t>
+  </si>
+  <si>
+    <t>Inicio milisegundos</t>
+  </si>
+  <si>
+    <t>Dia fin</t>
+  </si>
+  <si>
+    <t>Hora fin</t>
+  </si>
+  <si>
+    <t>Fin milisegundos</t>
+  </si>
+  <si>
+    <t>Pagado</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
+  </si>
+  <si>
+    <t>A pagar</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>2024-7-26</t>
+  </si>
+  <si>
+    <t>5:14:59 PM</t>
   </si>
   <si>
     <t>SCA1551</t>
   </si>
   <si>
-    <t>SBD6688</t>
-  </si>
-  <si>
-    <t>02:20:00 AM</t>
-  </si>
-  <si>
-    <t>fds</t>
-  </si>
-  <si>
-    <t>3:26:53 PM</t>
-  </si>
-  <si>
-    <t>ABC-1234</t>
-  </si>
-  <si>
-    <t>3:49:30 PM</t>
-  </si>
-  <si>
-    <t>CDE-9876</t>
-  </si>
-  <si>
-    <t>3:56:34 PM</t>
-  </si>
-  <si>
-    <t>pepe-134</t>
-  </si>
-  <si>
-    <t>4:06:44 PM</t>
-  </si>
-  <si>
-    <t>5:14:59 PM</t>
-  </si>
-  <si>
-    <t>2024-7-26</t>
-  </si>
-  <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>End date</t>
-  </si>
-  <si>
-    <t>Amount paid</t>
-  </si>
-  <si>
-    <t>Amount to be paid</t>
+    <t>2024-7-30</t>
+  </si>
+  <si>
+    <t>4:58:24 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -453,21 +443,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D8"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
   <cols>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,147 +471,90 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
+      <c r="E3">
+        <v>1722369504074</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Req 4 Print to thermal printer
</commit_message>
<xml_diff>
--- a/ElectronFrontend/assets/archivo.xlsx
+++ b/ElectronFrontend/assets/archivo.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Hoja 1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Otro" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Id</t>
   </si>
@@ -43,15 +44,15 @@
     <t>Pagado</t>
   </si>
   <si>
+    <t>A pagar</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
+  </si>
+  <si>
     <t>Tiempo</t>
   </si>
   <si>
-    <t>A pagar</t>
-  </si>
-  <si>
-    <t>Diferencia</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
@@ -68,6 +69,21 @@
   </si>
   <si>
     <t>4:58:24 PM</t>
+  </si>
+  <si>
+    <t>2024-7-31</t>
+  </si>
+  <si>
+    <t>SBD6688</t>
+  </si>
+  <si>
+    <t>11:49:32 AM</t>
+  </si>
+  <si>
+    <t>18 horas 51 minutos</t>
+  </si>
+  <si>
+    <t>11:20:41 AM</t>
   </si>
 </sst>
 </file>
@@ -444,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
@@ -536,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -551,10 +567,192 @@
       </c>
       <c r="E3">
         <v>1722369504074</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>1722369524074</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>1722437373229</v>
+      </c>
+      <c r="I4">
+        <v>1550</v>
+      </c>
+      <c r="J4">
+        <v>1520</v>
+      </c>
+      <c r="K4">
+        <v>-30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>1722369504074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>1722369524074</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>1722435642431</v>
+      </c>
+      <c r="I4">
+        <v>1500</v>
+      </c>
+      <c r="J4">
+        <v>1440</v>
+      </c>
+      <c r="K4">
+        <v>-60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Req 5 Testing and comment deletion
</commit_message>
<xml_diff>
--- a/ElectronFrontend/assets/archivo.xlsx
+++ b/ElectronFrontend/assets/archivo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Id</t>
   </si>
@@ -74,13 +74,43 @@
     <t>2024-7-31</t>
   </si>
   <si>
+    <t>12:48:57 PM</t>
+  </si>
+  <si>
+    <t>19 horas 51 minutos</t>
+  </si>
+  <si>
     <t>SBD6688</t>
   </si>
   <si>
-    <t>11:49:32 AM</t>
-  </si>
-  <si>
-    <t>18 horas 51 minutos</t>
+    <t>1:05:38 PM</t>
+  </si>
+  <si>
+    <t>20 horas 7 minutos</t>
+  </si>
+  <si>
+    <t>ABC1234</t>
+  </si>
+  <si>
+    <t>1:04:49 PM</t>
+  </si>
+  <si>
+    <t>fsd</t>
+  </si>
+  <si>
+    <t>1:22:10 PM</t>
+  </si>
+  <si>
+    <t>fddf</t>
+  </si>
+  <si>
+    <t>1:25:12 PM</t>
+  </si>
+  <si>
+    <t>2:02:40 PM</t>
+  </si>
+  <si>
+    <t>0 horas 37 minutos</t>
   </si>
   <si>
     <t>11:20:41 AM</t>
@@ -460,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="9.140625"/>
@@ -552,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -570,6 +600,24 @@
       </c>
       <c r="F3" t="s">
         <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>1722440938028</v>
+      </c>
+      <c r="I3">
+        <v>1600</v>
+      </c>
+      <c r="J3">
+        <v>1600</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -577,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -592,22 +640,94 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4">
-        <v>1722437373229</v>
+        <v>1722441938606</v>
       </c>
       <c r="I4">
-        <v>1550</v>
+        <v>1766</v>
       </c>
       <c r="J4">
-        <v>1520</v>
+        <v>1600</v>
       </c>
       <c r="K4">
-        <v>-30</v>
+        <v>-166</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>1722441889470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>1722442931280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>1722443112893</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>1722445360638</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>40</v>
+      </c>
+      <c r="K7">
+        <v>-10</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -722,7 +842,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -737,7 +857,7 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>1722435642431</v>

</xml_diff>